<commit_message>
ORCIDs added for Yousif and Javad
</commit_message>
<xml_diff>
--- a/dataset_description.xlsx
+++ b/dataset_description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bhavesh\Documents\GitHub\GI-review-dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417887B3-8A98-4739-A61F-B02BD7EC0A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72404373-6A5B-4B2F-B7A0-7563CCB762D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="1605" windowWidth="23760" windowHeight="13635" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
             <sz val="12"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>======
 ID#AAAADMZp7ig
@@ -171,12 +171,6 @@
     <t>https://orcid.org/0000-0001-5350-8156</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>https://orcid.org/0000-0002-5792-2845</t>
   </si>
   <si>
@@ -331,6 +325,12 @@
   </si>
   <si>
     <t>1.2.3</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-2628-4497</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-4444-3172</t>
   </si>
 </sst>
 </file>
@@ -340,7 +340,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -374,6 +374,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -817,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -964,248 +970,248 @@
         <v>36</v>
       </c>
       <c r="F6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="D7" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="E8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
         <v>51</v>
       </c>
-      <c r="F8" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" t="s">
-        <v>53</v>
-      </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" t="s">
-        <v>57</v>
-      </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>60</v>
       </c>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="D11" t="s">
         <v>62</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13"/>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>73</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="12">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C17" s="12">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>81</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>83</v>
       </c>
       <c r="D18"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>84</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>86</v>
       </c>
       <c r="D19"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>